<commit_message>
Created basic getCompanies function. Updated database model. Adjusted styles into dark theme.Adjusted formatting/spacing for subheaders and headers.
</commit_message>
<xml_diff>
--- a/docs/database_model.xlsx
+++ b/docs/database_model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A25B4D-C9C7-48DA-B8A2-149BCE3299C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5860F09-644F-4B4D-8DFF-90E89D698F0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{771582B4-90A9-40CA-BBD4-F5468E28D5A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>containers (Collection)</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>companies (Collection)</t>
+  </si>
+  <si>
+    <t>company_id</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>array of containers</t>
   </si>
 </sst>
 </file>
@@ -306,6 +318,59 @@
         <a:xfrm flipH="1">
           <a:off x="1162050" y="4692650"/>
           <a:ext cx="1384300" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1322916</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>70556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590903</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88195</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B2B86B8-3561-4E04-B8F5-1D257132CB9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2487083" y="4700764"/>
+          <a:ext cx="6447014" cy="1128889"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -631,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289D8918-7CC7-4091-A25E-52C3E725CE0F}">
-  <dimension ref="H26:L50"/>
+  <dimension ref="B26:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="72" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="72" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,34 +713,51 @@
     <col min="12" max="12" width="17.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="J26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="J27" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J28" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="J29" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="J30" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B31" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="J31" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="8:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add retrieval of transactions array from databases
</commit_message>
<xml_diff>
--- a/docs/database_model.xlsx
+++ b/docs/database_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5860F09-644F-4B4D-8DFF-90E89D698F0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B370223D-057D-430B-A750-8B3EFF3CD543}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{771582B4-90A9-40CA-BBD4-F5468E28D5A3}"/>
   </bookViews>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289D8918-7CC7-4091-A25E-52C3E725CE0F}">
   <dimension ref="B26:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="72" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>